<commit_message>
updating ETL steps doc
</commit_message>
<xml_diff>
--- a/Presentation/ETLSteps.xlsx
+++ b/Presentation/ETLSteps.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dhanaprakashdurairaj/Documents/GitHub/nba-player-analytics/Presentation/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dhanaprakashdurairaj/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{859733B1-9847-8E4C-A7EB-AEBD962AC3A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{F27A2010-4FAB-594E-A71E-2D856A58CCF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13080" yWindow="1780" windowWidth="20760" windowHeight="17940" xr2:uid="{2BA560AD-908E-F54F-AE67-AAC8640196EC}"/>
+    <workbookView xWindow="11800" yWindow="1920" windowWidth="20760" windowHeight="18680" xr2:uid="{2BA560AD-908E-F54F-AE67-AAC8640196EC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="40">
   <si>
     <t>S.No</t>
   </si>
@@ -84,45 +84,34 @@
 We wll not use the column for 2P%.</t>
   </si>
   <si>
-    <t>NBA STATs19-20.csv</t>
-  </si>
-  <si>
-    <t>Check whether player_id matches with stats data for 2016-19</t>
-  </si>
-  <si>
-    <t>Filter and keep only the players available in all seasons</t>
-  </si>
-  <si>
-    <t>NBA_salaries_2019_present.csv</t>
-  </si>
-  <si>
-    <t>Split playerid and playername</t>
-  </si>
-  <si>
-    <t>Check whether Salary is available for all players for each year 2016 to 2019
-a.	Only 415/436 rows have salary values 
-b.	2016-17: 436/436 unique playerids
-c.	2016-17: 498/498 unique playerids
-d.	2017-18: 474/474 unique playerids</t>
-  </si>
-  <si>
-    <t>Check whether Salary is available for all players</t>
-  </si>
-  <si>
-    <t>nba_stats_salaries_16-19.csv</t>
-  </si>
-  <si>
-    <t xml:space="preserve">only pick players for whom salary is available </t>
-  </si>
-  <si>
-    <t>cross checking files</t>
-  </si>
-  <si>
     <t>i.	2016-17: 486/595 players are unique
 ii.	2017-18: 540/664 players are unique
 iii.	2018-19: 530/708 players are unique
-iv.	2019-20: 529/651 players are unique
-v.	2019-20: 529/651 players are unique</t>
+iv.	2019-20: 529/651 players are unique</t>
+  </si>
+  <si>
+    <t>NBA STATs19-20.csv</t>
+  </si>
+  <si>
+    <t>Check whether player_id matches with stats data for 2016-19</t>
+  </si>
+  <si>
+    <t>Filter and keep only the players available in all seasons</t>
+  </si>
+  <si>
+    <t>NBA_salaries_2019_present.csv</t>
+  </si>
+  <si>
+    <t>Check whether Salary is available for all players</t>
+  </si>
+  <si>
+    <t>nba_stats_salaries_16-19.csv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">only pick players for whom salary is available </t>
+  </si>
+  <si>
+    <t>cross checking files</t>
   </si>
   <si>
     <t>merging documents</t>
@@ -140,9 +129,6 @@
 ii.	NBA_salaries_2019_present.csv</t>
   </si>
   <si>
-    <t xml:space="preserve">Spliting document into three tables </t>
-  </si>
-  <si>
     <t>NBA Players Stats 201819.csv
 NBA_salaries_2019_present.csv</t>
   </si>
@@ -166,16 +152,45 @@
   </si>
   <si>
     <t>Refer to ERD diagram</t>
+  </si>
+  <si>
+    <t>Check whether Salary is available for all players for each year 2016 to 2019
+a.	Only 415/436 rows have salary values 
+b.	2016-17: 436/436 unique playerids
+c.	2017-18: 498/498 unique playerids
+d.	2018-19: 474/474 unique playerids</t>
+  </si>
+  <si>
+    <t>2019-2020: Split playerid and playername</t>
+  </si>
+  <si>
+    <t>No Need to do this at pre-processing state</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Load data to player info table </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Load data to player stats table </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Load data to player salary table </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -191,6 +206,12 @@
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
       <name val="Helvetica Neue"/>
       <family val="2"/>
     </font>
@@ -236,7 +257,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -245,31 +266,42 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -588,12 +620,12 @@
   <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="19.83203125" customWidth="1"/>
+    <col min="2" max="2" width="31.83203125" customWidth="1"/>
     <col min="3" max="3" width="32.6640625" customWidth="1"/>
     <col min="4" max="4" width="67.33203125" style="1" customWidth="1"/>
     <col min="5" max="5" width="38.33203125" customWidth="1"/>
@@ -635,7 +667,7 @@
       <c r="E2" s="8"/>
       <c r="F2" s="2"/>
     </row>
-    <row r="3" spans="1:6" ht="102" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" ht="68" x14ac:dyDescent="0.2">
       <c r="A3" s="8">
         <v>2</v>
       </c>
@@ -649,7 +681,7 @@
         <v>10</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="F3" s="2"/>
     </row>
@@ -679,10 +711,10 @@
         <v>8</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D5" s="11" t="s">
-        <v>19</v>
+        <v>34</v>
       </c>
       <c r="E5" s="8"/>
       <c r="F5" s="2"/>
@@ -695,10 +727,10 @@
         <v>8</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>18</v>
+        <v>35</v>
       </c>
       <c r="E6" s="8"/>
       <c r="F6" s="2"/>
@@ -711,10 +743,10 @@
         <v>8</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E7" s="8"/>
       <c r="F7" s="2"/>
@@ -724,13 +756,13 @@
         <v>8</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
@@ -740,13 +772,13 @@
         <v>9</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
@@ -756,64 +788,66 @@
         <v>10</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D10" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E10" s="2"/>
+      <c r="D10" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>36</v>
+      </c>
       <c r="F10" s="2"/>
     </row>
     <row r="11" spans="1:6" ht="102" x14ac:dyDescent="0.2">
       <c r="A11" s="8">
         <v>12</v>
       </c>
-      <c r="B11" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="C11" s="9" t="s">
+      <c r="B11" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="D11" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="E11" s="8"/>
-      <c r="F11" s="2"/>
+      <c r="D11" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="E11" s="14"/>
+      <c r="F11" s="17"/>
     </row>
     <row r="12" spans="1:6" ht="68" x14ac:dyDescent="0.2">
       <c r="A12" s="8">
         <v>13</v>
       </c>
-      <c r="B12" s="8" t="s">
+      <c r="B12" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" s="18" t="s">
+        <v>26</v>
+      </c>
+      <c r="D12" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="C12" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="D12" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="E12" s="8"/>
-      <c r="F12" s="2"/>
+      <c r="E12" s="14"/>
+      <c r="F12" s="17"/>
     </row>
     <row r="13" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
         <v>15</v>
       </c>
       <c r="B13" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D13" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C13" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>31</v>
-      </c>
       <c r="E13" s="2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="F13" s="2"/>
     </row>
@@ -822,16 +856,16 @@
         <v>16</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D14" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E14" s="2" t="s">
         <v>33</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>36</v>
       </c>
       <c r="F14" s="2"/>
     </row>
@@ -840,16 +874,16 @@
         <v>17</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>28</v>
+        <v>39</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="F15" s="2"/>
     </row>

</xml_diff>

<commit_message>
Starting to check-in changes for preprocessing of data
</commit_message>
<xml_diff>
--- a/Presentation/ETLSteps.xlsx
+++ b/Presentation/ETLSteps.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dhanaprakashdurairaj/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dhanaprakashdurairaj/Documents/GitHub/nba-player-analytics/Presentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F27A2010-4FAB-594E-A71E-2D856A58CCF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46B044A3-CCCC-3245-9765-CED0F61E20D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11800" yWindow="1920" windowWidth="20760" windowHeight="18680" xr2:uid="{2BA560AD-908E-F54F-AE67-AAC8640196EC}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="35840" windowHeight="22400" xr2:uid="{2BA560AD-908E-F54F-AE67-AAC8640196EC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="42">
   <si>
     <t>S.No</t>
   </si>
@@ -174,6 +174,12 @@
   </si>
   <si>
     <t xml:space="preserve">Load data to player salary table </t>
+  </si>
+  <si>
+    <t>Not Needed</t>
+  </si>
+  <si>
+    <t>Noit Needed</t>
   </si>
 </sst>
 </file>
@@ -289,9 +295,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -301,6 +304,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -620,7 +626,7 @@
   <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -629,6 +635,7 @@
     <col min="3" max="3" width="32.6640625" customWidth="1"/>
     <col min="4" max="4" width="67.33203125" style="1" customWidth="1"/>
     <col min="5" max="5" width="38.33203125" customWidth="1"/>
+    <col min="6" max="6" width="13" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="17" x14ac:dyDescent="0.2">
@@ -793,7 +800,7 @@
       <c r="C10" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D10" s="13" t="s">
+      <c r="D10" s="18" t="s">
         <v>21</v>
       </c>
       <c r="E10" s="6" t="s">
@@ -805,33 +812,37 @@
       <c r="A11" s="8">
         <v>12</v>
       </c>
-      <c r="B11" s="14" t="s">
+      <c r="B11" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="C11" s="15" t="s">
+      <c r="C11" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="D11" s="16" t="s">
+      <c r="D11" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="E11" s="14"/>
-      <c r="F11" s="17"/>
+      <c r="E11" s="13"/>
+      <c r="F11" s="16" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="12" spans="1:6" ht="68" x14ac:dyDescent="0.2">
       <c r="A12" s="8">
         <v>13</v>
       </c>
-      <c r="B12" s="14" t="s">
+      <c r="B12" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="C12" s="18" t="s">
+      <c r="C12" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="D12" s="16" t="s">
+      <c r="D12" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="E12" s="14"/>
-      <c r="F12" s="17"/>
+      <c r="E12" s="13"/>
+      <c r="F12" s="16" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="13" spans="1:6" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" s="2">

</xml_diff>

<commit_message>
Prepocessing Player Stats for year 2019-20
</commit_message>
<xml_diff>
--- a/Presentation/ETLSteps.xlsx
+++ b/Presentation/ETLSteps.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dhanaprakashdurairaj/Documents/GitHub/nba-player-analytics/Presentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46B044A3-CCCC-3245-9765-CED0F61E20D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3F9AD7C-C84E-0847-9A0F-43848D1CB1F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="35840" windowHeight="22400" xr2:uid="{2BA560AD-908E-F54F-AE67-AAC8640196EC}"/>
+    <workbookView xWindow="6160" yWindow="1980" windowWidth="20760" windowHeight="18680" xr2:uid="{2BA560AD-908E-F54F-AE67-AAC8640196EC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="43">
   <si>
     <t>S.No</t>
   </si>
@@ -180,6 +180,9 @@
   </si>
   <si>
     <t>Noit Needed</t>
+  </si>
+  <si>
+    <t>Completed</t>
   </si>
 </sst>
 </file>
@@ -625,8 +628,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83DE458D-2BAD-3A49-A7CD-9C9D058C973C}">
   <dimension ref="A1:F15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -672,7 +675,9 @@
         <v>7</v>
       </c>
       <c r="E2" s="8"/>
-      <c r="F2" s="2"/>
+      <c r="F2" s="2" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="3" spans="1:6" ht="68" x14ac:dyDescent="0.2">
       <c r="A3" s="8">
@@ -690,7 +695,9 @@
       <c r="E3" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="F3" s="2"/>
+      <c r="F3" s="2" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="4" spans="1:6" ht="68" x14ac:dyDescent="0.2">
       <c r="A4" s="8">
@@ -708,7 +715,9 @@
       <c r="E4" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="F4" s="2"/>
+      <c r="F4" s="2" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="5" spans="1:6" ht="85" x14ac:dyDescent="0.2">
       <c r="A5" s="8">

</xml_diff>